<commit_message>
Updated for EA 23.252 Stable. Added an optional Night Vision (Cat’s Eye) feature that automatically grants Night Vision at night.
EA 23.252 Stable に対応しました。夜間に自動で暗視（猫の目）を付与するオプションを追加しました。

已更新至 EA 23.252 Stable。新增可选的夜间夜视（猫之眼）功能，在夜晚自动赋予夜视效果。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -197,6 +197,30 @@
   </si>
   <si>
     <t xml:space="preserve">移除蝙蝠变形的冷却时间。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Night Vision At Night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">夜間に暗視を有効にする</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用夜间夜视</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grants Night Vision (Cat's Eye) automatically while it is night.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">夜間になると自動的に暗視（猫の目）を付与します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在夜间自动赋予夜视（猫之眼）效果。</t>
   </si>
 </sst>
 </file>
@@ -206,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -233,6 +257,11 @@
       <name val="Noto Sans SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -277,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,6 +320,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -417,10 +450,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,6 +675,34 @@
         <v>57</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>